<commit_message>
implemented data driven test
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -1,68 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>admin@yourstore.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>adm</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>admin12</t>
-  </si>
-  <si>
-    <t>admin@</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <color theme="1"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
@@ -72,25 +38,87 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -288,74 +316,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.5"/>
+    <col width="17.5" customWidth="1" style="2" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>exp</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>admin@yourstore.com</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>admin@yourstore.com</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>adm</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>admin@yourstore.com</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>admin12</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>admin@yourstore.com</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>admin@</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>